<commit_message>
Use multiplier/overhead in benchmark plots
</commit_message>
<xml_diff>
--- a/doc/benchmarks.xlsx
+++ b/doc/benchmarks.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niels\Code\luigi\koffi\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F1CCE4-C41A-48E7-BB42-29C7FFCAA406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81A1386-335F-41AA-9539-1F74B5B10F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="2460" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
+    <workbookView xWindow="1995" yWindow="1545" windowWidth="21600" windowHeight="11385" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
   </bookViews>
   <sheets>
     <sheet name="Linux" sheetId="1" r:id="rId1"/>
-    <sheet name="Windows" sheetId="3" r:id="rId2"/>
+    <sheet name="Windows" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
   <si>
     <t>Test</t>
   </si>
@@ -59,19 +59,55 @@
     <t>NAPI</t>
   </si>
   <si>
-    <t>C++</t>
-  </si>
-  <si>
     <t xml:space="preserve">    </t>
   </si>
   <si>
     <t>rand</t>
   </si>
   <si>
-    <t xml:space="preserve">        </t>
+    <t xml:space="preserve">      </t>
   </si>
   <si>
-    <t xml:space="preserve">      </t>
+    <t>node-ffi</t>
+  </si>
+  <si>
+    <t>(ref)</t>
+  </si>
+  <si>
+    <t>× 1.81</t>
+  </si>
+  <si>
+    <t>× 75</t>
+  </si>
+  <si>
+    <t>× 1.71</t>
+  </si>
+  <si>
+    <t>× 1.18</t>
+  </si>
+  <si>
+    <t>× 3.28</t>
+  </si>
+  <si>
+    <t>× 233</t>
+  </si>
+  <si>
+    <t>× 42</t>
+  </si>
+  <si>
+    <t>× 1.84</t>
+  </si>
+  <si>
+    <t>× 1.99</t>
+  </si>
+  <si>
+    <t>× 161</t>
+  </si>
+  <si>
+    <t>× 1.23</t>
+  </si>
+  <si>
+    <t>× 3.7</t>
   </si>
 </sst>
 </file>
@@ -146,10 +182,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="108"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="8"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -217,7 +253,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="1"/>
         <c:ser>
@@ -241,7 +277,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent6">
+                  <a:shade val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -260,7 +298,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent6">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -279,7 +319,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent6">
+                  <a:shade val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -298,7 +340,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent6">
+                  <a:shade val="70000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -317,7 +361,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent6">
+                  <a:shade val="80000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -336,7 +382,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent6">
+                  <a:shade val="90000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -355,7 +403,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -374,7 +422,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent6">
+                  <a:tint val="90000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -393,8 +443,8 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
+                <a:schemeClr val="accent6">
+                  <a:tint val="80000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
@@ -414,7 +464,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent6">
+                  <a:tint val="70000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -433,8 +485,8 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
+                <a:schemeClr val="accent6">
+                  <a:tint val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
@@ -448,8 +500,493 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:tint val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000016-EA4C-4BBF-ABC4-8B3290ECEFD2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:tint val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-BED7-48FD-8840-D485E65131F2}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:dLbls>
-            <c:numFmt formatCode="0.00" sourceLinked="0"/>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C635741D-E8AE-4B06-AEAF-3C71CFEFC12E}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{C635741D-E8AE-4B06-AEAF-3C71CFEFC12E}</c15:txfldGUID>
+                      <c15:f>Linux!$D$3</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>(ref)</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-8325-4B73-8F13-CE0999669DCD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{934F11AF-2B39-43E5-A43B-455F76AA0F8B}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{934F11AF-2B39-43E5-A43B-455F76AA0F8B}</c15:txfldGUID>
+                      <c15:f>Linux!$D$4</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>× 1.81</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-8325-4B73-8F13-CE0999669DCD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                    <a:spAutoFit/>
+                  </a:bodyPr>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:fld id="{C331D300-4736-48D2-86F4-6F9D61335651}" type="CELLREF">
+                      <a:rPr lang="en-US" sz="1600"/>
+                      <a:pPr>
+                        <a:defRPr sz="1600" b="1"/>
+                      </a:pPr>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                  <a:spAutoFit/>
+                </a:bodyPr>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="75000"/>
+                          <a:lumOff val="25000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{C331D300-4736-48D2-86F4-6F9D61335651}</c15:txfldGUID>
+                      <c15:f>Linux!$D$5</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>× 75</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-8325-4B73-8F13-CE0999669DCD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{AE42DE83-9114-4161-A4D3-8843A5D164E3}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{AE42DE83-9114-4161-A4D3-8843A5D164E3}</c15:txfldGUID>
+                      <c15:f>Linux!$D$7</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>(ref)</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-8325-4B73-8F13-CE0999669DCD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FE72684A-A58C-4FB1-BEAF-9A1259CE7F1E}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{FE72684A-A58C-4FB1-BEAF-9A1259CE7F1E}</c15:txfldGUID>
+                      <c15:f>Linux!$D$8</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>× 1.71</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-8325-4B73-8F13-CE0999669DCD}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{36599ABC-BCF4-40B8-A64F-A8E08F8C29E3}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{36599ABC-BCF4-40B8-A64F-A8E08F8C29E3}</c15:txfldGUID>
+                      <c15:f>Linux!$D$9</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>× 233</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-694B-4FA3-9D3E-7A389C7F3B40}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1862E73A-BDB9-4CBF-A8D7-07CEEBE080E7}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{1862E73A-BDB9-4CBF-A8D7-07CEEBE080E7}</c15:txfldGUID>
+                      <c15:f>Linux!$D$11</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>(ref)</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-694B-4FA3-9D3E-7A389C7F3B40}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0D109535-746F-49EE-974C-E4B85DDD3943}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{0D109535-746F-49EE-974C-E4B85DDD3943}</c15:txfldGUID>
+                      <c15:f>Linux!$D$12</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>× 1.18</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-089F-4D94-A25D-9B748D43B1F9}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{5AE41765-C6B2-4990-8ACE-32F4EBAF5D09}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{5AE41765-C6B2-4990-8ACE-32F4EBAF5D09}</c15:txfldGUID>
+                      <c15:f>Linux!$D$13</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>× 3.28</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000016-EA4C-4BBF-ABC4-8B3290ECEFD2}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="General" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -464,7 +1001,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -509,9 +1046,9 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Linux!$A$2:$B$12</c:f>
+              <c:f>Linux!$A$2:$B$14</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="1">
                     <c:v>NAPI</c:v>
@@ -519,36 +1056,42 @@
                   <c:pt idx="2">
                     <c:v>Koffi</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="3">
+                    <c:v>node-ffi</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>NAPI</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>Koffi</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>C++</c:v>
+                    <c:v>node-ffi</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
                     <c:v>NAPI</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="10">
                     <c:v>Koffi</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>node-ffi</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="1">
                     <c:v>rand</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="4">
                     <c:v>      </c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>atoi</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="8">
                     <c:v>    </c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="9">
                     <c:v>raylib</c:v>
                   </c:pt>
                 </c:lvl>
@@ -557,30 +1100,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Linux!$C$2:$C$12</c:f>
+              <c:f>Linux!$C$2:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="1">
-                  <c:v>1.44</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6</c:v>
+                  <c:v>1.81</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.97</c:v>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.07</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.71</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.31</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.9</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.86</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -601,17 +1150,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:overlap val="-76"/>
         <c:axId val="1638056304"/>
         <c:axId val="1638056720"/>
       </c:barChart>
       <c:catAx>
         <c:axId val="1638056304"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -629,7 +1177,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -649,16 +1197,16 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="0"/>
-        <c:tickLblSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="1638056720"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -677,11 +1225,11 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -694,17 +1242,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1400"/>
-                  <a:t>Execution</a:t>
+                  <a:rPr lang="fr-FR" sz="1600"/>
+                  <a:t>Overhead compared to reference implementation (log10 scale)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="fr-FR" sz="1400" baseline="0"/>
-                  <a:t> time (sec)</a:t>
-                </a:r>
-                <a:endParaRPr lang="fr-FR" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.10729816060129466"/>
+              <c:y val="0.11003477059386176"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -714,11 +1265,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -737,7 +1288,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="high"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -828,10 +1379,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="106"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="6"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -899,7 +1450,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="1"/>
         <c:ser>
@@ -923,7 +1474,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent4">
+                  <a:shade val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -932,7 +1485,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-2C72-4E1F-B433-E7A432A3DDB6}"/>
+                <c16:uniqueId val="{00000001-B9BB-485C-850D-8C294307D416}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -942,7 +1495,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4">
+                  <a:shade val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -951,7 +1506,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-2C72-4E1F-B433-E7A432A3DDB6}"/>
+                <c16:uniqueId val="{00000003-B9BB-485C-850D-8C294307D416}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -961,7 +1516,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent4">
+                  <a:shade val="60000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -970,7 +1527,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000005-2C72-4E1F-B433-E7A432A3DDB6}"/>
+                <c16:uniqueId val="{00000005-B9BB-485C-850D-8C294307D416}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -980,7 +1537,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent4">
+                  <a:shade val="70000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -989,7 +1548,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000007-2C72-4E1F-B433-E7A432A3DDB6}"/>
+                <c16:uniqueId val="{00000007-B9BB-485C-850D-8C294307D416}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -999,7 +1558,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent4">
+                  <a:shade val="80000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1008,7 +1569,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000009-2C72-4E1F-B433-E7A432A3DDB6}"/>
+                <c16:uniqueId val="{00000009-B9BB-485C-850D-8C294307D416}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1018,7 +1579,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent4">
+                  <a:shade val="90000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1027,7 +1590,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000B-2C72-4E1F-B433-E7A432A3DDB6}"/>
+                <c16:uniqueId val="{0000000B-B9BB-485C-850D-8C294307D416}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1046,7 +1609,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000D-2C72-4E1F-B433-E7A432A3DDB6}"/>
+                <c16:uniqueId val="{0000000D-B9BB-485C-850D-8C294307D416}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1056,7 +1619,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="accent4">
+                  <a:tint val="90000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1065,7 +1630,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000F-1684-4D18-AEFB-932EC1DAA794}"/>
+                <c16:uniqueId val="{0000000F-B9BB-485C-850D-8C294307D416}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1075,8 +1640,8 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
+                <a:schemeClr val="accent4">
+                  <a:tint val="80000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
@@ -1086,7 +1651,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000011-1684-4D18-AEFB-932EC1DAA794}"/>
+                <c16:uniqueId val="{00000011-B9BB-485C-850D-8C294307D416}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1096,7 +1661,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent4">
+                  <a:tint val="70000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1105,7 +1672,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000013-1684-4D18-AEFB-932EC1DAA794}"/>
+                <c16:uniqueId val="{00000013-B9BB-485C-850D-8C294307D416}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -1115,8 +1682,8 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
+                <a:schemeClr val="accent4">
+                  <a:tint val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln>
@@ -1126,12 +1693,450 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000015-3DE0-4557-8B05-2F8B752031ED}"/>
+                <c16:uniqueId val="{00000015-B9BB-485C-850D-8C294307D416}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:tint val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-B9BB-485C-850D-8C294307D416}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:tint val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-B9BB-485C-850D-8C294307D416}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:dLbls>
-            <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C635741D-E8AE-4B06-AEAF-3C71CFEFC12E}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{C635741D-E8AE-4B06-AEAF-3C71CFEFC12E}</c15:txfldGUID>
+                      <c15:f>Windows!$D$3</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>(ref)</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-B9BB-485C-850D-8C294307D416}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{934F11AF-2B39-43E5-A43B-455F76AA0F8B}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{934F11AF-2B39-43E5-A43B-455F76AA0F8B}</c15:txfldGUID>
+                      <c15:f>Windows!$D$4</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>× 1.84</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-B9BB-485C-850D-8C294307D416}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{C331D300-4736-48D2-86F4-6F9D61335651}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{C331D300-4736-48D2-86F4-6F9D61335651}</c15:txfldGUID>
+                      <c15:f>Windows!$D$5</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>× 42</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-B9BB-485C-850D-8C294307D416}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{AE42DE83-9114-4161-A4D3-8843A5D164E3}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{AE42DE83-9114-4161-A4D3-8843A5D164E3}</c15:txfldGUID>
+                      <c15:f>Windows!$D$7</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>(ref)</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000B-B9BB-485C-850D-8C294307D416}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FE72684A-A58C-4FB1-BEAF-9A1259CE7F1E}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{FE72684A-A58C-4FB1-BEAF-9A1259CE7F1E}</c15:txfldGUID>
+                      <c15:f>Windows!$D$8</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>× 1.99</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-B9BB-485C-850D-8C294307D416}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{36599ABC-BCF4-40B8-A64F-A8E08F8C29E3}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{36599ABC-BCF4-40B8-A64F-A8E08F8C29E3}</c15:txfldGUID>
+                      <c15:f>Windows!$D$9</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>× 161</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-B9BB-485C-850D-8C294307D416}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="9"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1862E73A-BDB9-4CBF-A8D7-07CEEBE080E7}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{1862E73A-BDB9-4CBF-A8D7-07CEEBE080E7}</c15:txfldGUID>
+                      <c15:f>Windows!$D$11</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>(ref)</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-B9BB-485C-850D-8C294307D416}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="10"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{0D109535-746F-49EE-974C-E4B85DDD3943}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{0D109535-746F-49EE-974C-E4B85DDD3943}</c15:txfldGUID>
+                      <c15:f>Windows!$D$12</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>× 1.23</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-B9BB-485C-850D-8C294307D416}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{5AE41765-C6B2-4990-8ACE-32F4EBAF5D09}" type="CELLREF">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[REFCELL]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="fr-FR"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable>
+                    <c15:dlblFTEntry>
+                      <c15:txfldGUID>{5AE41765-C6B2-4990-8ACE-32F4EBAF5D09}</c15:txfldGUID>
+                      <c15:f>Windows!$D$13</c15:f>
+                      <c15:dlblFieldTableCache>
+                        <c:ptCount val="1"/>
+                        <c:pt idx="0">
+                          <c:v>× 3.7</c:v>
+                        </c:pt>
+                      </c15:dlblFieldTableCache>
+                    </c15:dlblFTEntry>
+                  </c15:dlblFieldTable>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000017-B9BB-485C-850D-8C294307D416}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:numFmt formatCode="General" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1146,7 +2151,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -1191,9 +2196,9 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Windows!$A$2:$B$12</c:f>
+              <c:f>Windows!$A$2:$B$14</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="12"/>
                 <c:lvl>
                   <c:pt idx="1">
                     <c:v>NAPI</c:v>
@@ -1201,36 +2206,42 @@
                   <c:pt idx="2">
                     <c:v>Koffi</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="3">
+                    <c:v>node-ffi</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>NAPI</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="6">
                     <c:v>Koffi</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>C++</c:v>
+                    <c:v>node-ffi</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="9">
                     <c:v>NAPI</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="10">
                     <c:v>Koffi</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>node-ffi</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="1">
                     <c:v>rand</c:v>
                   </c:pt>
-                  <c:pt idx="3">
-                    <c:v>        </c:v>
+                  <c:pt idx="4">
+                    <c:v>      </c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="5">
                     <c:v>atoi</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="8">
                     <c:v>    </c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="9">
                     <c:v>raylib</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1239,37 +2250,43 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Windows!$C$2:$C$12</c:f>
+              <c:f>Windows!$C$2:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="1">
-                  <c:v>2.1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.87</c:v>
+                  <c:v>1.84</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.97</c:v>
+                <c:pt idx="3">
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.91</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.99</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.67</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>12.05</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.84</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.23</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000E-2C72-4E1F-B433-E7A432A3DDB6}"/>
+              <c16:uniqueId val="{0000001A-B9BB-485C-850D-8C294307D416}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1283,17 +2300,16 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:overlap val="-76"/>
         <c:axId val="1638056304"/>
         <c:axId val="1638056720"/>
       </c:barChart>
       <c:catAx>
         <c:axId val="1638056304"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1311,7 +2327,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1336,10 +2352,11 @@
       <c:valAx>
         <c:axId val="1638056720"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="t"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1358,11 +2375,11 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1375,17 +2392,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1400"/>
-                  <a:t>Execution</a:t>
+                  <a:rPr lang="fr-FR" sz="1600"/>
+                  <a:t>Overhead compared to reference implementation (log10 scale)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="fr-FR" sz="1400" baseline="0"/>
-                  <a:t> time (sec)</a:t>
-                </a:r>
-                <a:endParaRPr lang="fr-FR" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.10729816060129466"/>
+              <c:y val="0.11003477059386176"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1395,11 +2415,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1418,7 +2438,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="high"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -1431,7 +2451,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1503,82 +2523,14 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="19">
   <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="17">
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -2593,15 +3545,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>761998</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2633,23 +3585,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B30BF077-1343-454E-B533-C52DE62B54E0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44B8B5C6-6010-4E1C-A26A-5645BACF9A61}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2969,15 +3921,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CCB824-727A-454B-9045-C9B1F28AEFCD}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2988,92 +3940,137 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="3">
-        <v>1.44</v>
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3">
-        <v>2.6</v>
+        <v>1.81</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3">
+        <v>75</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1">
+        <v>233</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
-        <v>2.97</v>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
-        <v>5.07</v>
+      <c r="C12" s="1">
+        <v>1.18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1">
-        <v>9.31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1">
-        <v>10.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1">
-        <v>12.86</v>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -3084,16 +4081,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4F65A5A-B90B-422E-8A40-1C68FD816CAE}">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF254FDB-3299-431D-8033-6BEFA204D913}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3104,92 +4101,137 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.84</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
-        <v>2.1</v>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
-        <v>3.87</v>
+      <c r="C8" s="1">
+        <v>1.99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
+      <c r="C9" s="1">
+        <v>161</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="1">
-        <v>2.97</v>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="1">
-        <v>5.91</v>
+      <c r="C12" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1">
-        <v>10.67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1">
-        <v>12.05</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1">
-        <v>14.84</v>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use relative performance in benchmark plots
</commit_message>
<xml_diff>
--- a/doc/benchmarks.xlsx
+++ b/doc/benchmarks.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niels\Code\luigi\koffi\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81A1386-335F-41AA-9539-1F74B5B10F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D6ABC98-F5E8-426D-A480-8C573C3AB2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="1545" windowWidth="21600" windowHeight="11385" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
+    <workbookView xWindow="1995" yWindow="1545" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
   </bookViews>
   <sheets>
     <sheet name="Linux" sheetId="1" r:id="rId1"/>
     <sheet name="Windows" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,77 +44,77 @@
     <t>Variant</t>
   </si>
   <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>rand</t>
+  </si>
+  <si>
+    <t>NAPI</t>
+  </si>
+  <si>
+    <t>× 1 (ref)</t>
+  </si>
+  <si>
+    <t>Koffi</t>
+  </si>
+  <si>
+    <t>× 0.55</t>
+  </si>
+  <si>
+    <t>node-ffi</t>
+  </si>
+  <si>
+    <t>× 0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
     <t>atoi</t>
+  </si>
+  <si>
+    <t>× 0.58</t>
+  </si>
+  <si>
+    <t>× 0.005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
   <si>
     <t>raylib</t>
   </si>
   <si>
-    <t>Time</t>
+    <t>× 0.85</t>
   </si>
   <si>
-    <t>Koffi</t>
+    <t>× 0.30</t>
   </si>
   <si>
-    <t>NAPI</t>
+    <t>× 0.54</t>
   </si>
   <si>
-    <t xml:space="preserve">    </t>
+    <t>× 0.02</t>
   </si>
   <si>
-    <t>rand</t>
+    <t>× 0.50</t>
   </si>
   <si>
-    <t xml:space="preserve">      </t>
+    <t>× 0.006</t>
   </si>
   <si>
-    <t>node-ffi</t>
+    <t>× 0.81</t>
   </si>
   <si>
-    <t>(ref)</t>
-  </si>
-  <si>
-    <t>× 1.81</t>
-  </si>
-  <si>
-    <t>× 75</t>
-  </si>
-  <si>
-    <t>× 1.71</t>
-  </si>
-  <si>
-    <t>× 1.18</t>
-  </si>
-  <si>
-    <t>× 3.28</t>
-  </si>
-  <si>
-    <t>× 233</t>
-  </si>
-  <si>
-    <t>× 42</t>
-  </si>
-  <si>
-    <t>× 1.84</t>
-  </si>
-  <si>
-    <t>× 1.99</t>
-  </si>
-  <si>
-    <t>× 161</t>
-  </si>
-  <si>
-    <t>× 1.23</t>
-  </si>
-  <si>
-    <t>× 3.7</t>
+    <t>× 0.27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,13 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -196,7 +195,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -209,14 +208,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1600"/>
-              <a:t>Linux x86_64</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Linux x86_64 (AMD® Ryzen™ 7 4700U)</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" baseline="0"/>
-              <a:t> (AMD® Ryzen™ 7 4700U)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1600"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -233,7 +227,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -245,7 +239,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -553,9 +547,9 @@
                     <a:fld id="{C635741D-E8AE-4B06-AEAF-3C71CFEFC12E}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -575,7 +569,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>(ref)</c:v>
+                          <c:v>× 1 (ref)</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -597,9 +591,9 @@
                     <a:fld id="{934F11AF-2B39-43E5-A43B-455F76AA0F8B}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -619,7 +613,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 1.81</c:v>
+                          <c:v>× 0.55</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -635,65 +629,18 @@
               <c:idx val="3"/>
               <c:tx>
                 <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                    <a:spAutoFit/>
-                  </a:bodyPr>
+                  <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
                     <a:fld id="{C331D300-4736-48D2-86F4-6F9D61335651}" type="CELLREF">
                       <a:rPr lang="en-US" sz="1600"/>
-                      <a:pPr>
-                        <a:defRPr sz="1600" b="1"/>
-                      </a:pPr>
-                      <a:t>[REFCELL]</a:t>
+                      <a:pPr/>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="fr-FR"/>
-                </a:p>
-              </c:txPr>
               <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
@@ -710,7 +657,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 75</c:v>
+                          <c:v>× 0.01</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -732,9 +679,9 @@
                     <a:fld id="{AE42DE83-9114-4161-A4D3-8843A5D164E3}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -754,7 +701,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>(ref)</c:v>
+                          <c:v>× 1 (ref)</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -776,9 +723,9 @@
                     <a:fld id="{FE72684A-A58C-4FB1-BEAF-9A1259CE7F1E}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -798,7 +745,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 1.71</c:v>
+                          <c:v>× 0.58</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -820,9 +767,9 @@
                     <a:fld id="{36599ABC-BCF4-40B8-A64F-A8E08F8C29E3}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -842,7 +789,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 233</c:v>
+                          <c:v>× 0.005</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -864,9 +811,9 @@
                     <a:fld id="{1862E73A-BDB9-4CBF-A8D7-07CEEBE080E7}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -886,7 +833,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>(ref)</c:v>
+                          <c:v>× 1 (ref)</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -908,9 +855,9 @@
                     <a:fld id="{0D109535-746F-49EE-974C-E4B85DDD3943}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -930,7 +877,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 1.18</c:v>
+                          <c:v>× 0.85</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -952,9 +899,9 @@
                     <a:fld id="{5AE41765-C6B2-4990-8ACE-32F4EBAF5D09}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -974,7 +921,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 3.28</c:v>
+                          <c:v>× 0.30</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1013,7 +960,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1108,28 +1055,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.81</c:v>
+                  <c:v>0.5524861878453039</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>75</c:v>
+                  <c:v>1.3333333333333334E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.71</c:v>
+                  <c:v>0.58479532163742687</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>233</c:v>
+                  <c:v>4.2918454935622317E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.18</c:v>
+                  <c:v>0.84745762711864414</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.28</c:v>
+                  <c:v>0.3048780487804878</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1189,7 +1136,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1638056720"/>
@@ -1202,8 +1149,8 @@
       <c:valAx>
         <c:axId val="1638056720"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
+          <c:max val="1.2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -1242,20 +1189,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1600"/>
-                  <a:t>Overhead compared to reference implementation (log10 scale)</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Relative performance of each implementation</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.10729816060129466"/>
-              <c:y val="0.11003477059386176"/>
-            </c:manualLayout>
-          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1281,7 +1220,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1313,7 +1252,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1638056304"/>
@@ -1361,7 +1300,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1393,7 +1332,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1406,14 +1345,9 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1600"/>
-              <a:t>Windows x86_64</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Windows x86_64 (Intel® Core™ i5-4460)</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1600" baseline="0"/>
-              <a:t> (Intel® Core™ i5-4460)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1600"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1430,7 +1364,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1442,7 +1376,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1750,9 +1684,9 @@
                     <a:fld id="{C635741D-E8AE-4B06-AEAF-3C71CFEFC12E}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1772,7 +1706,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>(ref)</c:v>
+                          <c:v>× 1 (ref)</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1794,9 +1728,9 @@
                     <a:fld id="{934F11AF-2B39-43E5-A43B-455F76AA0F8B}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1816,7 +1750,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 1.84</c:v>
+                          <c:v>× 0.54</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1838,9 +1772,9 @@
                     <a:fld id="{C331D300-4736-48D2-86F4-6F9D61335651}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1860,7 +1794,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 42</c:v>
+                          <c:v>× 0.02</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1882,9 +1816,9 @@
                     <a:fld id="{AE42DE83-9114-4161-A4D3-8843A5D164E3}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1904,7 +1838,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>(ref)</c:v>
+                          <c:v>× 1 (ref)</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1926,9 +1860,9 @@
                     <a:fld id="{FE72684A-A58C-4FB1-BEAF-9A1259CE7F1E}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1948,7 +1882,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 1.99</c:v>
+                          <c:v>× 0.50</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1970,9 +1904,9 @@
                     <a:fld id="{36599ABC-BCF4-40B8-A64F-A8E08F8C29E3}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1992,7 +1926,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 161</c:v>
+                          <c:v>× 0.006</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -2014,9 +1948,9 @@
                     <a:fld id="{1862E73A-BDB9-4CBF-A8D7-07CEEBE080E7}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2036,7 +1970,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>(ref)</c:v>
+                          <c:v>× 1 (ref)</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -2058,9 +1992,9 @@
                     <a:fld id="{0D109535-746F-49EE-974C-E4B85DDD3943}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2080,7 +2014,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 1.23</c:v>
+                          <c:v>× 0.81</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -2102,9 +2036,9 @@
                     <a:fld id="{5AE41765-C6B2-4990-8ACE-32F4EBAF5D09}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[REFCELL]</a:t>
+                      <a:t>[]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="fr-FR"/>
+                    <a:endParaRPr/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2124,7 +2058,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 3.7</c:v>
+                          <c:v>× 0.27</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -2163,7 +2097,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="fr-FR"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -2258,28 +2192,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.84</c:v>
+                  <c:v>0.54347826086956519</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42</c:v>
+                  <c:v>2.3809523809523808E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.99</c:v>
+                  <c:v>0.50251256281407031</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>161</c:v>
+                  <c:v>6.2111801242236021E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.23</c:v>
+                  <c:v>0.81300813008130079</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.7</c:v>
+                  <c:v>0.27027027027027023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2339,7 +2273,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1638056720"/>
@@ -2352,7 +2286,6 @@
       <c:valAx>
         <c:axId val="1638056720"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2392,20 +2325,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="fr-FR" sz="1600"/>
-                  <a:t>Overhead compared to reference implementation (log10 scale)</a:t>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Relative performance of each implementation</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.10729816060129466"/>
-              <c:y val="0.11003477059386176"/>
-            </c:manualLayout>
-          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2431,7 +2356,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="fr-FR"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2463,7 +2388,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1638056304"/>
@@ -2511,7 +2436,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3545,15 +3470,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
+      <xdr:colOff>752474</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3586,15 +3511,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
+      <xdr:colOff>752474</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3625,7 +3550,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3923,13 +3848,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CCB824-727A-454B-9045-C9B1F28AEFCD}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3937,140 +3862,146 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2"/>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <f>1/1.81</f>
+        <v>0.5524861878453039</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2"/>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
+      <c r="C5">
+        <f>1/75</f>
+        <v>1.3333333333333334E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.81</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="3">
-        <v>75</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>1.71</v>
+        <f>1/1.71</f>
+        <v>0.58479532163742687</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>233</v>
+        <f>1/233</f>
+        <v>4.2918454935622317E-3</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1">
-        <v>1.18</v>
+        <f>1/1.18</f>
+        <v>0.84745762711864414</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1">
-        <v>3.28</v>
+        <f>1/3.28</f>
+        <v>0.3048780487804878</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -4084,13 +4015,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF254FDB-3299-431D-8033-6BEFA204D913}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4098,137 +4029,143 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2"/>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <f>1/1.84</f>
+        <v>0.54347826086956519</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2"/>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
+      <c r="C5">
+        <f>1/42</f>
+        <v>2.3809523809523808E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.84</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="3">
-        <v>42</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>1.99</v>
+        <f>1/1.99</f>
+        <v>0.50251256281407031</v>
       </c>
       <c r="D8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>161</v>
+        <f>1/161</f>
+        <v>6.2111801242236021E-3</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="1">
-        <v>1.23</v>
+        <f>1/1.23</f>
+        <v>0.81300813008130079</v>
       </c>
       <c r="D12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1">
-        <v>3.7</v>
+        <f>1/3.7</f>
+        <v>0.27027027027027023</v>
       </c>
       <c r="D13" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Update benchmarks with Clang builds data
</commit_message>
<xml_diff>
--- a/doc/benchmarks.xlsx
+++ b/doc/benchmarks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niels\Code\luigi\koffi\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D6ABC98-F5E8-426D-A480-8C573C3AB2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB1C9CC-9720-4513-A150-8A8F4930F72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="1545" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
   </bookViews>
   <sheets>
     <sheet name="Linux" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>Test</t>
   </si>
@@ -59,13 +59,7 @@
     <t>Koffi</t>
   </si>
   <si>
-    <t>× 0.55</t>
-  </si>
-  <si>
     <t>node-ffi</t>
-  </si>
-  <si>
-    <t>× 0.01</t>
   </si>
   <si>
     <t xml:space="preserve">      </t>
@@ -77,44 +71,47 @@
     <t>× 0.58</t>
   </si>
   <si>
-    <t>× 0.005</t>
-  </si>
-  <si>
     <t xml:space="preserve">    </t>
   </si>
   <si>
     <t>raylib</t>
   </si>
   <si>
-    <t>× 0.85</t>
-  </si>
-  <si>
-    <t>× 0.30</t>
-  </si>
-  <si>
-    <t>× 0.54</t>
-  </si>
-  <si>
     <t>× 0.02</t>
-  </si>
-  <si>
-    <t>× 0.50</t>
   </si>
   <si>
     <t>× 0.006</t>
   </si>
   <si>
-    <t>× 0.81</t>
+    <t>× 0.27</t>
   </si>
   <si>
-    <t>× 0.27</t>
+    <t>× 0.68</t>
+  </si>
+  <si>
+    <t>× 0.66</t>
+  </si>
+  <si>
+    <t>× 0.004</t>
+  </si>
+  <si>
+    <t>× 0.83</t>
+  </si>
+  <si>
+    <t>× 0.76</t>
+  </si>
+  <si>
+    <t>× 0.82</t>
+  </si>
+  <si>
+    <t>× 0.23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,7 +236,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -547,9 +544,9 @@
                     <a:fld id="{C635741D-E8AE-4B06-AEAF-3C71CFEFC12E}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -591,9 +588,9 @@
                     <a:fld id="{934F11AF-2B39-43E5-A43B-455F76AA0F8B}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -613,7 +610,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.55</c:v>
+                          <c:v>× 0.68</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -635,9 +632,9 @@
                     <a:fld id="{C331D300-4736-48D2-86F4-6F9D61335651}" type="CELLREF">
                       <a:rPr lang="en-US" sz="1600"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -657,7 +654,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.01</c:v>
+                          <c:v>× 0.02</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -679,9 +676,9 @@
                     <a:fld id="{AE42DE83-9114-4161-A4D3-8843A5D164E3}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -723,9 +720,9 @@
                     <a:fld id="{FE72684A-A58C-4FB1-BEAF-9A1259CE7F1E}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -745,7 +742,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.58</c:v>
+                          <c:v>× 0.66</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -767,9 +764,9 @@
                     <a:fld id="{36599ABC-BCF4-40B8-A64F-A8E08F8C29E3}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -789,7 +786,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.005</c:v>
+                          <c:v>× 0.004</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -811,9 +808,9 @@
                     <a:fld id="{1862E73A-BDB9-4CBF-A8D7-07CEEBE080E7}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -855,9 +852,9 @@
                     <a:fld id="{0D109535-746F-49EE-974C-E4B85DDD3943}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -877,7 +874,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.85</c:v>
+                          <c:v>× 0.83</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -899,9 +896,9 @@
                     <a:fld id="{5AE41765-C6B2-4990-8ACE-32F4EBAF5D09}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -921,7 +918,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.30</c:v>
+                          <c:v>× 0.27</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -960,7 +957,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1055,28 +1052,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5524861878453039</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3333333333333334E-2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.58479532163742687</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.2918454935622317E-3</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.84745762711864414</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.3048780487804878</c:v>
+                  <c:v>0.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1136,7 +1133,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1638056720"/>
@@ -1220,7 +1217,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1252,7 +1249,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1638056304"/>
@@ -1300,7 +1297,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1376,7 +1373,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1684,9 +1681,9 @@
                     <a:fld id="{C635741D-E8AE-4B06-AEAF-3C71CFEFC12E}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1728,9 +1725,9 @@
                     <a:fld id="{934F11AF-2B39-43E5-A43B-455F76AA0F8B}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1750,7 +1747,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.54</c:v>
+                          <c:v>× 0.76</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1772,9 +1769,9 @@
                     <a:fld id="{C331D300-4736-48D2-86F4-6F9D61335651}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1816,9 +1813,9 @@
                     <a:fld id="{AE42DE83-9114-4161-A4D3-8843A5D164E3}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1860,9 +1857,9 @@
                     <a:fld id="{FE72684A-A58C-4FB1-BEAF-9A1259CE7F1E}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1882,7 +1879,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.50</c:v>
+                          <c:v>× 0.58</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1904,9 +1901,9 @@
                     <a:fld id="{36599ABC-BCF4-40B8-A64F-A8E08F8C29E3}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1948,9 +1945,9 @@
                     <a:fld id="{1862E73A-BDB9-4CBF-A8D7-07CEEBE080E7}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -1992,9 +1989,9 @@
                     <a:fld id="{0D109535-746F-49EE-974C-E4B85DDD3943}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2014,7 +2011,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.81</c:v>
+                          <c:v>× 0.82</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -2036,9 +2033,9 @@
                     <a:fld id="{5AE41765-C6B2-4990-8ACE-32F4EBAF5D09}" type="CELLREF">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
-                      <a:t>[]</a:t>
+                      <a:t>[REFCELL]</a:t>
                     </a:fld>
-                    <a:endParaRPr/>
+                    <a:endParaRPr lang="fr-FR"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2058,7 +2055,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.27</c:v>
+                          <c:v>× 0.23</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -2097,7 +2094,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -2192,28 +2189,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.54347826086956519</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3809523809523808E-2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.50251256281407031</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.2111801242236021E-3</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.81300813008130079</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.27027027027027023</c:v>
+                  <c:v>0.23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2273,7 +2270,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1638056720"/>
@@ -2356,7 +2353,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="fr-FR"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2388,7 +2385,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1638056304"/>
@@ -2436,7 +2433,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3550,7 +3547,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3848,13 +3845,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CCB824-727A-454B-9045-C9B1F28AEFCD}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3865,12 +3862,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3884,42 +3881,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4">
-        <f>1/1.81</f>
-        <v>0.5524861878453039</v>
+        <v>0.68</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>0.02</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C5">
-        <f>1/75</f>
-        <v>1.3333333333333334E-2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -3931,42 +3926,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <f>1/1.71</f>
-        <v>0.58479532163742687</v>
+        <v>0.66</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
-        <f>1/233</f>
-        <v>4.2918454935622317E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -3978,30 +3971,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="1">
-        <f>1/1.18</f>
-        <v>0.84745762711864414</v>
+        <v>0.83</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1">
-        <f>1/3.28</f>
-        <v>0.3048780487804878</v>
+        <v>0.27</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -4015,13 +4006,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF254FDB-3299-431D-8033-6BEFA204D913}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4032,12 +4023,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4051,42 +4042,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4">
-        <f>1/1.84</f>
-        <v>0.54347826086956519</v>
+        <v>0.76</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>0.02</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C5">
-        <f>1/42</f>
-        <v>2.3809523809523808E-2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
@@ -4098,42 +4087,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <f>1/1.99</f>
-        <v>0.50251256281407031</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
-        <f>1/161</f>
-        <v>6.2111801242236021E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -4145,30 +4132,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="1">
-        <f>1/1.23</f>
-        <v>0.81300813008130079</v>
+        <v>0.82</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1">
-        <f>1/3.7</f>
-        <v>0.27027027027027023</v>
+        <v>0.23</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automate production of benchmark markdown tables
</commit_message>
<xml_diff>
--- a/doc/benchmarks.xlsx
+++ b/doc/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niels\Code\luigi\koffi\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB1C9CC-9720-4513-A150-8A8F4930F72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F945D24A-1C46-4B32-B16A-A71BE35315B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
   </bookViews>
   <sheets>
     <sheet name="Linux" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
   <si>
     <t>Test</t>
   </si>
@@ -68,43 +68,10 @@
     <t>atoi</t>
   </si>
   <si>
-    <t>× 0.58</t>
-  </si>
-  <si>
     <t xml:space="preserve">    </t>
   </si>
   <si>
     <t>raylib</t>
-  </si>
-  <si>
-    <t>× 0.02</t>
-  </si>
-  <si>
-    <t>× 0.006</t>
-  </si>
-  <si>
-    <t>× 0.27</t>
-  </si>
-  <si>
-    <t>× 0.68</t>
-  </si>
-  <si>
-    <t>× 0.66</t>
-  </si>
-  <si>
-    <t>× 0.004</t>
-  </si>
-  <si>
-    <t>× 0.83</t>
-  </si>
-  <si>
-    <t>× 0.76</t>
-  </si>
-  <si>
-    <t>× 0.82</t>
-  </si>
-  <si>
-    <t>× 0.23</t>
   </si>
 </sst>
 </file>
@@ -3845,8 +3812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CCB824-727A-454B-9045-C9B1F28AEFCD}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3889,8 +3856,9 @@
       <c r="C4">
         <v>0.68</v>
       </c>
-      <c r="D4" t="s">
-        <v>16</v>
+      <c r="D4" t="str">
+        <f>_xlfn.CONCAT("× ", SUBSTITUTE(C4, ",", "."))</f>
+        <v>× 0.68</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3901,8 +3869,9 @@
       <c r="C5">
         <v>0.02</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
+      <c r="D5" t="str">
+        <f>_xlfn.CONCAT("× ", SUBSTITUTE(C5, ",", "."))</f>
+        <v>× 0.02</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3934,8 +3903,9 @@
       <c r="C8" s="1">
         <v>0.66</v>
       </c>
-      <c r="D8" t="s">
-        <v>17</v>
+      <c r="D8" t="str">
+        <f>_xlfn.CONCAT("× ", SUBSTITUTE(C8, ",", "."))</f>
+        <v>× 0.66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3946,20 +3916,21 @@
       <c r="C9" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D9" t="s">
-        <v>18</v>
+      <c r="D9" t="str">
+        <f>_xlfn.CONCAT("× ", SUBSTITUTE(C9, ",", "."))</f>
+        <v>× 0.004</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -3979,8 +3950,9 @@
       <c r="C12" s="1">
         <v>0.83</v>
       </c>
-      <c r="D12" t="s">
-        <v>19</v>
+      <c r="D12" t="str">
+        <f>_xlfn.CONCAT("× ", SUBSTITUTE(C12, ",", "."))</f>
+        <v>× 0.83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3991,8 +3963,9 @@
       <c r="C13" s="1">
         <v>0.27</v>
       </c>
-      <c r="D13" t="s">
-        <v>15</v>
+      <c r="D13" t="str">
+        <f>_xlfn.CONCAT("× ", SUBSTITUTE(C13, ",", "."))</f>
+        <v>× 0.27</v>
       </c>
     </row>
   </sheetData>
@@ -4006,8 +3979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF254FDB-3299-431D-8033-6BEFA204D913}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4050,8 +4023,9 @@
       <c r="C4">
         <v>0.76</v>
       </c>
-      <c r="D4" t="s">
-        <v>20</v>
+      <c r="D4" t="str">
+        <f>_xlfn.CONCAT("× ", SUBSTITUTE(C4, ",", "."))</f>
+        <v>× 0.76</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4062,8 +4036,9 @@
       <c r="C5">
         <v>0.02</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
+      <c r="D5" t="str">
+        <f>_xlfn.CONCAT("× ", SUBSTITUTE(C5, ",", "."))</f>
+        <v>× 0.02</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4095,8 +4070,9 @@
       <c r="C8" s="1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="D8" t="s">
-        <v>10</v>
+      <c r="D8" t="str">
+        <f>_xlfn.CONCAT("× ", SUBSTITUTE(C8, ",", "."))</f>
+        <v>× 0.58</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4107,20 +4083,21 @@
       <c r="C9" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="D9" t="s">
-        <v>14</v>
+      <c r="D9" t="str">
+        <f>_xlfn.CONCAT("× ", SUBSTITUTE(C9, ",", "."))</f>
+        <v>× 0.006</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>4</v>
@@ -4140,8 +4117,9 @@
       <c r="C12" s="1">
         <v>0.82</v>
       </c>
-      <c r="D12" t="s">
-        <v>21</v>
+      <c r="D12" t="str">
+        <f>_xlfn.CONCAT("× ", SUBSTITUTE(C12, ",", "."))</f>
+        <v>× 0.82</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -4152,8 +4130,9 @@
       <c r="C13" s="1">
         <v>0.23</v>
       </c>
-      <c r="D13" t="s">
-        <v>22</v>
+      <c r="D13" t="str">
+        <f>_xlfn.CONCAT("× ", SUBSTITUTE(C13, ",", "."))</f>
+        <v>× 0.23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Koffi benchmark results
</commit_message>
<xml_diff>
--- a/doc/benchmarks.xlsx
+++ b/doc/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niels\Code\luigi\koffi\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F945D24A-1C46-4B32-B16A-A71BE35315B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE00DE2-EF5F-4597-A322-C3F1AE8E7A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
+    <workbookView xWindow="-25140" yWindow="1395" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
   </bookViews>
   <sheets>
     <sheet name="Linux" sheetId="1" r:id="rId1"/>
@@ -709,7 +709,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.66</c:v>
+                          <c:v>× 0.62</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -753,7 +753,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.004</c:v>
+                          <c:v>× 0.009</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -885,7 +885,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.27</c:v>
+                          <c:v>× 0.28</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1028,10 +1028,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.66</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.0000000000000001E-3</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -1040,7 +1040,7 @@
                   <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.27</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1714,7 +1714,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.76</c:v>
+                          <c:v>× 0.77</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1846,7 +1846,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.58</c:v>
+                          <c:v>× 0.62</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1890,7 +1890,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.006</c:v>
+                          <c:v>× 0.009</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -1978,7 +1978,7 @@
                       <c15:dlblFieldTableCache>
                         <c:ptCount val="1"/>
                         <c:pt idx="0">
-                          <c:v>× 0.82</c:v>
+                          <c:v>× 0.83</c:v>
                         </c:pt>
                       </c15:dlblFieldTableCache>
                     </c15:dlblFTEntry>
@@ -2156,7 +2156,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.02</c:v>
@@ -2165,16 +2165,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.0000000000000001E-3</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.82</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.23</c:v>
@@ -3812,8 +3812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CCB824-727A-454B-9045-C9B1F28AEFCD}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3901,11 +3901,11 @@
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>0.66</v>
+        <v>0.62</v>
       </c>
       <c r="D8" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C8, ",", "."))</f>
-        <v>× 0.66</v>
+        <v>× 0.62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3914,11 +3914,11 @@
         <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>4.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="D9" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C9, ",", "."))</f>
-        <v>× 0.004</v>
+        <v>× 0.009</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -3961,11 +3961,11 @@
         <v>7</v>
       </c>
       <c r="C13" s="1">
-        <v>0.27</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D13" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C13, ",", "."))</f>
-        <v>× 0.27</v>
+        <v>× 0.28</v>
       </c>
     </row>
   </sheetData>
@@ -3979,8 +3979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF254FDB-3299-431D-8033-6BEFA204D913}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4021,11 +4021,11 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
       <c r="D4" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C4, ",", "."))</f>
-        <v>× 0.76</v>
+        <v>× 0.77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4068,11 +4068,11 @@
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.62</v>
       </c>
       <c r="D8" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C8, ",", "."))</f>
-        <v>× 0.58</v>
+        <v>× 0.62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4081,11 +4081,11 @@
         <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>6.0000000000000001E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="D9" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C9, ",", "."))</f>
-        <v>× 0.006</v>
+        <v>× 0.009</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4115,11 +4115,11 @@
         <v>6</v>
       </c>
       <c r="C12" s="1">
-        <v>0.82</v>
+        <v>0.83</v>
       </c>
       <c r="D12" t="str">
         <f>_xlfn.CONCAT("× ", SUBSTITUTE(C12, ",", "."))</f>
-        <v>× 0.82</v>
+        <v>× 0.83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix title in Linux benchmark graphs
</commit_message>
<xml_diff>
--- a/doc/benchmarks.xlsx
+++ b/doc/benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niels\Code\luigi\koffi\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE00DE2-EF5F-4597-A322-C3F1AE8E7A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF045003-0C7F-4D2C-8FEB-B06692CC30B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25140" yWindow="1395" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{A2D128F3-7EA7-4666-84BF-881211D61592}"/>
   </bookViews>
   <sheets>
     <sheet name="Linux" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,17 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Linux x86_64 (AMD® Ryzen™ 7 4700U)</a:t>
+              <a:t>Linux x86_64 (</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Intel® Core™ i5-4460</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3812,8 +3822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CCB824-727A-454B-9045-C9B1F28AEFCD}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3979,7 +3989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF254FDB-3299-431D-8033-6BEFA204D913}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>

</xml_diff>